<commit_message>
fixing mapping and inStrain queues
</commit_message>
<xml_diff>
--- a/metadata/Danish_FullScale_WWTPs/selected-metagenomes.xlsx
+++ b/metadata/Danish_FullScale_WWTPs/selected-metagenomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcdaniel/Desktop/McMahon-Lab/EBPR-Projects/AcDiv/metadata/Danish_FullScale_WWTPs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACC9FCD2-E666-9C40-BA7A-2DFEDAC583D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71251B42-4BB3-A943-953F-335924195DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="1020" windowWidth="26840" windowHeight="15000" xr2:uid="{3C19988E-8429-534F-BD46-452D9C7C288A}"/>
+    <workbookView xWindow="1960" yWindow="1020" windowWidth="26840" windowHeight="15000" xr2:uid="{3C19988E-8429-534F-BD46-452D9C7C288A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -669,26 +669,27 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B22"/>
+      <selection activeCell="F1" sqref="F1:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1">
-        <v>43342</v>
+        <v>43341</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>69</v>
@@ -696,16 +697,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>43341</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>70</v>
@@ -713,33 +714,33 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
-        <v>43341</v>
+        <v>43342</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>66</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>43350</v>
+        <v>43341</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>72</v>
@@ -747,16 +748,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>43341</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>73</v>
@@ -764,16 +765,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>43341</v>
+        <v>43340</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
@@ -781,16 +782,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
         <v>43341</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>75</v>
@@ -798,16 +799,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>43341</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>76</v>
@@ -815,16 +816,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1">
-        <v>43341</v>
+        <v>43350</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
         <v>77</v>
@@ -832,16 +833,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>43341</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>78</v>
@@ -849,16 +850,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>43341</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
@@ -866,16 +867,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1">
-        <v>43346</v>
+        <v>43341</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
         <v>80</v>
@@ -900,16 +901,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
-        <v>43341</v>
+        <v>43346</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>82</v>
@@ -917,16 +918,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>43341</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
         <v>83</v>
@@ -934,16 +935,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1">
         <v>43341</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
         <v>84</v>
@@ -951,16 +952,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1">
-        <v>43350</v>
+        <v>43341</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
         <v>85</v>
@@ -968,16 +969,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1">
         <v>43341</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
         <v>86</v>
@@ -985,16 +986,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1">
         <v>43341</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
         <v>87</v>
@@ -1002,16 +1003,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1">
         <v>43341</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
         <v>88</v>
@@ -1019,16 +1020,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1">
-        <v>43340</v>
+        <v>43350</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
         <v>89</v>
@@ -1036,41 +1037,41 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1">
         <v>43341</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
+      <c r="A23" t="s">
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1">
         <v>43341</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D26">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D23">
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>